<commit_message>
Properly understanding the current rotation of reels when they stop, just need to correspond the 10 results to the symbols and then calculate payout. froze reels from rotating in y and z axes because a 1-time bug occurred where 1 reel started doing crazy wobbles.
</commit_message>
<xml_diff>
--- a/SlotMachine/Stats/PayoutInfo.xlsx
+++ b/SlotMachine/Stats/PayoutInfo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Reel Position</t>
   </si>
@@ -114,6 +114,39 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>if y = 180, sub all by 180</t>
+  </si>
+  <si>
+    <t>use x - 180</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -477,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +524,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -499,87 +532,179 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="M8">
+        <v>-90</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -593,7 +718,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>777</v>
       </c>
@@ -608,7 +733,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -623,7 +748,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Game now calculates and pays out credits if the player wins. Need to adjust how interactionsController checks though.
</commit_message>
<xml_diff>
--- a/SlotMachine/Stats/PayoutInfo.xlsx
+++ b/SlotMachine/Stats/PayoutInfo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Reel Position</t>
   </si>
@@ -114,39 +114,6 @@
   </si>
   <si>
     <t>Total:</t>
-  </si>
-  <si>
-    <t>if y = 180, sub all by 180</t>
-  </si>
-  <si>
-    <t>use x - 180</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -190,12 +157,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +493,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -532,179 +501,165 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="6">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
         <v>16</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="6">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5">
         <v>17</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="6">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
         <v>18</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="6">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5">
         <v>19</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
         <v>10</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
         <v>11</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="M8">
-        <v>-90</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="6">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5">
         <v>13</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5">
         <v>14</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5">
         <v>15</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -718,7 +673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>777</v>
       </c>
@@ -733,7 +688,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -748,7 +703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Machine now pays out credits. Will make dispense coins next instead. Working on adjusting payouts to be close to fair.
</commit_message>
<xml_diff>
--- a/SlotMachine/Stats/PayoutInfo.xlsx
+++ b/SlotMachine/Stats/PayoutInfo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Reel Position</t>
   </si>
@@ -68,24 +68,6 @@
     <t>aaa</t>
   </si>
   <si>
-    <t>_ _ c</t>
-  </si>
-  <si>
-    <t>_ c _</t>
-  </si>
-  <si>
-    <t>c _ _</t>
-  </si>
-  <si>
-    <t>_cc</t>
-  </si>
-  <si>
-    <t>c_c</t>
-  </si>
-  <si>
-    <t>cc_</t>
-  </si>
-  <si>
     <t>Heart</t>
   </si>
   <si>
@@ -114,6 +96,18 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Return:</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -145,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -153,11 +147,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -165,6 +221,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +557,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -501,12 +565,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6">
         <v>6</v>
@@ -517,7 +581,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -533,7 +597,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -549,12 +613,12 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6">
         <v>9</v>
@@ -565,7 +629,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -581,7 +645,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -597,12 +661,12 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -613,7 +677,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -629,12 +693,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6">
         <v>4</v>
@@ -645,7 +709,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -659,7 +723,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -667,13 +731,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>777</v>
       </c>
@@ -688,99 +752,102 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>10</v>
+        <v>4.1152263374485596</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D29" si="0">(1000/C15)*B15</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D15:D25" si="0">(1000/C15)*B15</f>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2">
-        <v>10</v>
+        <v>12.345679012345679</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>50</v>
@@ -793,24 +860,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2">
         <v>1000</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>35</v>
@@ -823,109 +890,56 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2">
         <v>1000</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2">
         <v>1000</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10">
+        <f>SUM(D14:D25)</f>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>35</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>35</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29">
-        <v>35</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3">
-        <f>SUM(D14:D29)</f>
-        <v>995</v>
-      </c>
-      <c r="E30">
-        <f>D30/10</f>
-        <v>99.5</v>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14">
+        <f>D26/1000</f>
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed payouts. Payouts can now be set from unity interface.
</commit_message>
<xml_diff>
--- a/SlotMachine/Stats/PayoutInfo.xlsx
+++ b/SlotMachine/Stats/PayoutInfo.xlsx
@@ -114,6 +114,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="&quot;1:&quot;#"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,7 +219,6 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -229,6 +231,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,7 +549,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,10 +561,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -572,10 +575,10 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>6</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>16</v>
       </c>
       <c r="E2" s="1"/>
@@ -588,10 +591,10 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>7</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>17</v>
       </c>
       <c r="E3" s="1"/>
@@ -604,10 +607,10 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>8</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>18</v>
       </c>
       <c r="E4" s="1"/>
@@ -620,10 +623,10 @@
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>9</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>19</v>
       </c>
       <c r="E5" s="1"/>
@@ -636,10 +639,10 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>10</v>
       </c>
       <c r="E6" s="1"/>
@@ -652,10 +655,10 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>11</v>
       </c>
       <c r="E7" s="1"/>
@@ -668,10 +671,10 @@
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
@@ -684,10 +687,10 @@
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>13</v>
       </c>
       <c r="E9" s="1"/>
@@ -700,10 +703,10 @@
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>14</v>
       </c>
       <c r="E10" s="1"/>
@@ -716,24 +719,24 @@
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
         <v>15</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -742,14 +745,14 @@
         <v>777</v>
       </c>
       <c r="B14">
-        <v>200</v>
-      </c>
-      <c r="C14" s="2">
+        <v>100</v>
+      </c>
+      <c r="C14" s="14">
         <v>1000</v>
       </c>
       <c r="D14">
         <f>(1000/C14)*B14</f>
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -759,7 +762,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="14">
         <v>4.1152263374485596</v>
       </c>
       <c r="D15">
@@ -772,14 +775,14 @@
         <v>26</v>
       </c>
       <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="14">
         <v>12.345679012345679</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>324</v>
       </c>
       <c r="J16" t="s">
         <v>27</v>
@@ -792,7 +795,7 @@
       <c r="B17">
         <v>50</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="14">
         <v>1000</v>
       </c>
       <c r="D17">
@@ -805,14 +808,14 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2">
+        <v>20</v>
+      </c>
+      <c r="C18" s="14">
         <v>1000</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,7 +825,7 @@
       <c r="B19">
         <v>35</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="14">
         <v>1000</v>
       </c>
       <c r="D19">
@@ -835,14 +838,14 @@
         <v>12</v>
       </c>
       <c r="B20">
-        <v>45</v>
-      </c>
-      <c r="C20" s="2">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14">
         <v>1000</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,14 +853,14 @@
         <v>13</v>
       </c>
       <c r="B21">
-        <v>50</v>
-      </c>
-      <c r="C21" s="2">
+        <v>45</v>
+      </c>
+      <c r="C21" s="14">
         <v>1000</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -867,7 +870,7 @@
       <c r="B22">
         <v>35</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="14">
         <v>1000</v>
       </c>
       <c r="D22">
@@ -882,7 +885,7 @@
       <c r="B23">
         <v>35</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="14">
         <v>1000</v>
       </c>
       <c r="D23">
@@ -897,7 +900,7 @@
       <c r="B24">
         <v>35</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="14">
         <v>1000</v>
       </c>
       <c r="D24">
@@ -912,7 +915,7 @@
       <c r="B25">
         <v>35</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="14">
         <v>1000</v>
       </c>
       <c r="D25">
@@ -921,25 +924,25 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10">
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9">
         <f>SUM(D14:D25)</f>
-        <v>950</v>
+        <v>997</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14">
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13">
         <f>D26/1000</f>
-        <v>0.95</v>
+        <v>0.997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>